<commit_message>
DLSV2-600 Updates tests to handle new spreadsheet column
</commit_message>
<xml_diff>
--- a/DigitalLearningSolutions.Data.Tests/TestData/CourseDelegateExportAllDataDownloadTest.xlsx
+++ b/DigitalLearningSolutions.Data.Tests/TestData/CourseDelegateExportAllDataDownloadTest.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alejac\Git\DLSV2\DigitalLearningSolutions.Data.Tests\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\digitallearningsolutions\DigitalLearningSolutions.Data.Tests\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E960CAC4-91AD-4E06-86D0-8B84EA23C627}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEC1E2C1-860C-4241-912C-02864BCADB45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23136" yWindow="-96" windowWidth="23232" windowHeight="13992" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28898" yWindow="2835" windowWidth="28996" windowHeight="15795" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Course Delegates" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="44">
   <si>
     <t>Last name</t>
   </si>
@@ -145,10 +145,13 @@
     <t>Admin field 3</t>
   </si>
   <si>
-    <t>Course One</t>
-  </si>
-  <si>
-    <t>Course Two</t>
+    <t>Course name</t>
+  </si>
+  <si>
+    <t>Course One - v1</t>
+  </si>
+  <si>
+    <t>Course Two - v1</t>
   </si>
 </sst>
 </file>
@@ -158,7 +161,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -176,6 +179,11 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -227,10 +235,11 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:X9" totalsRowShown="0">
-  <autoFilter ref="A1:X9" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <tableColumns count="24">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Last name"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:Y9" totalsRowShown="0">
+  <autoFilter ref="A1:Y9" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <tableColumns count="25">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Course name"/>
+    <tableColumn id="25" xr3:uid="{1B2F547F-6999-4B23-8184-4D24ED626D1A}" name="Last name"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="First name"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Email"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Role type"/>
@@ -544,157 +553,164 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:X9"/>
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:Y9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" outlineLevelRow="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.28515625" customWidth="1"/>
-    <col min="2" max="2" width="13.5703125" customWidth="1"/>
-    <col min="3" max="3" width="17" customWidth="1"/>
-    <col min="4" max="4" width="47.85546875" customWidth="1"/>
-    <col min="5" max="5" width="18.28515625" customWidth="1"/>
-    <col min="6" max="6" width="28.28515625" customWidth="1"/>
-    <col min="7" max="7" width="13.85546875" customWidth="1"/>
-    <col min="8" max="8" width="27.5703125" customWidth="1"/>
-    <col min="9" max="9" width="14.42578125" customWidth="1"/>
-    <col min="10" max="11" width="19.85546875" customWidth="1"/>
-    <col min="12" max="12" width="15.28515625" customWidth="1"/>
-    <col min="13" max="13" width="19.85546875" customWidth="1"/>
-    <col min="14" max="14" width="9.85546875" customWidth="1"/>
-    <col min="15" max="15" width="17.42578125" customWidth="1"/>
-    <col min="16" max="16" width="18.42578125" customWidth="1"/>
-    <col min="17" max="17" width="21.7109375" customWidth="1"/>
-    <col min="18" max="18" width="12.28515625" customWidth="1"/>
-    <col min="19" max="19" width="9.85546875" customWidth="1"/>
-    <col min="20" max="20" width="16.85546875" customWidth="1"/>
-    <col min="21" max="21" width="10.5703125" customWidth="1"/>
-    <col min="22" max="22" width="20.85546875" customWidth="1"/>
-    <col min="23" max="23" width="14.28515625" customWidth="1"/>
-    <col min="24" max="24" width="11.85546875" customWidth="1"/>
+    <col min="1" max="2" width="13.26953125" customWidth="1"/>
+    <col min="3" max="3" width="13.54296875" customWidth="1"/>
+    <col min="4" max="4" width="17" customWidth="1"/>
+    <col min="5" max="5" width="47.81640625" customWidth="1"/>
+    <col min="6" max="6" width="18.26953125" customWidth="1"/>
+    <col min="7" max="7" width="28.26953125" customWidth="1"/>
+    <col min="8" max="8" width="13.81640625" customWidth="1"/>
+    <col min="9" max="9" width="27.54296875" customWidth="1"/>
+    <col min="10" max="10" width="14.453125" customWidth="1"/>
+    <col min="11" max="12" width="19.81640625" customWidth="1"/>
+    <col min="13" max="13" width="15.26953125" customWidth="1"/>
+    <col min="14" max="14" width="19.81640625" customWidth="1"/>
+    <col min="15" max="15" width="9.81640625" customWidth="1"/>
+    <col min="16" max="16" width="17.453125" customWidth="1"/>
+    <col min="17" max="17" width="18.453125" customWidth="1"/>
+    <col min="18" max="18" width="21.7265625" customWidth="1"/>
+    <col min="19" max="19" width="12.26953125" customWidth="1"/>
+    <col min="20" max="20" width="9.81640625" customWidth="1"/>
+    <col min="21" max="21" width="16.81640625" customWidth="1"/>
+    <col min="22" max="22" width="10.54296875" customWidth="1"/>
+    <col min="23" max="23" width="20.81640625" customWidth="1"/>
+    <col min="24" max="24" width="14.26953125" customWidth="1"/>
+    <col min="25" max="25" width="11.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>41</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>38</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>39</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="J2" s="4"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="4"/>
-      <c r="M2" s="3"/>
-      <c r="S2" s="2"/>
-      <c r="U2" s="2"/>
+        <v>42</v>
+      </c>
+      <c r="B2" s="5"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="4"/>
+      <c r="N2" s="3"/>
+      <c r="T2" s="2"/>
+      <c r="V2" s="2"/>
     </row>
-    <row r="3" spans="1:24" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" t="s">
         <v>21</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>22</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>23</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>24</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>25</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>26</v>
       </c>
-      <c r="J3" s="4">
+      <c r="K3" s="4">
         <v>41053</v>
       </c>
-      <c r="K3" s="3">
+      <c r="L3" s="3">
         <v>43167</v>
       </c>
-      <c r="L3" s="4"/>
-      <c r="M3" s="3"/>
-      <c r="N3">
+      <c r="M3" s="4"/>
+      <c r="N3" s="3"/>
+      <c r="O3">
         <v>2</v>
       </c>
-      <c r="O3">
-        <v>0</v>
-      </c>
       <c r="P3">
         <v>0</v>
       </c>
@@ -704,153 +720,163 @@
       <c r="R3">
         <v>0</v>
       </c>
-      <c r="S3" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="U3" s="2" t="b">
+      <c r="S3">
+        <v>0</v>
+      </c>
+      <c r="T3" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="V3" s="2" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:24" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B4" t="s">
         <v>27</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>28</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>30</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>31</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>32</v>
       </c>
-      <c r="J4" s="4">
+      <c r="K4" s="4">
         <v>40443</v>
       </c>
-      <c r="K4" s="4">
+      <c r="L4" s="4">
         <v>43167</v>
       </c>
-      <c r="L4" s="4"/>
-      <c r="M4" s="3">
+      <c r="M4" s="4"/>
+      <c r="N4" s="3">
         <v>43167</v>
       </c>
-      <c r="N4">
+      <c r="O4">
         <v>2</v>
       </c>
-      <c r="O4">
-        <v>0</v>
-      </c>
       <c r="P4">
         <v>0</v>
       </c>
       <c r="Q4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R4">
+        <v>1</v>
+      </c>
+      <c r="S4">
         <v>100</v>
       </c>
-      <c r="S4" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="U4" s="2" t="b">
+      <c r="T4" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="V4" s="2" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:24" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:25" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B5" t="s">
         <v>33</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>34</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>35</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>36</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>25</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
         <v>37</v>
       </c>
-      <c r="J5" s="4">
+      <c r="K5" s="4">
         <v>40624</v>
       </c>
-      <c r="K5" s="4">
+      <c r="L5" s="4">
         <v>43167</v>
       </c>
-      <c r="L5" s="4"/>
-      <c r="M5" s="3">
+      <c r="M5" s="4"/>
+      <c r="N5" s="3">
         <v>43167</v>
       </c>
-      <c r="N5">
-        <v>1</v>
-      </c>
       <c r="O5">
         <v>1</v>
       </c>
       <c r="P5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R5">
+        <v>1</v>
+      </c>
+      <c r="S5">
         <v>100</v>
       </c>
-      <c r="S5" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="U5" s="2" t="b">
+      <c r="T5" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="V5" s="2" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
-        <v>42</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="B6" s="5"/>
     </row>
-    <row r="7" spans="1:24" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:25" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B7" t="s">
         <v>21</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>22</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>23</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>24</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>25</v>
       </c>
-      <c r="I7" t="s">
+      <c r="J7" t="s">
         <v>26</v>
       </c>
-      <c r="J7" s="4">
+      <c r="K7" s="4">
         <v>41053</v>
       </c>
-      <c r="K7" s="3">
+      <c r="L7" s="3">
         <v>43167</v>
       </c>
-      <c r="L7" s="4"/>
-      <c r="M7" s="3"/>
-      <c r="N7">
+      <c r="M7" s="4"/>
+      <c r="N7" s="3"/>
+      <c r="O7">
         <v>2</v>
       </c>
-      <c r="O7">
-        <v>0</v>
-      </c>
       <c r="P7">
         <v>0</v>
       </c>
@@ -860,76 +886,83 @@
       <c r="R7">
         <v>0</v>
       </c>
-      <c r="S7" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="U7" s="2" t="b">
+      <c r="S7">
+        <v>0</v>
+      </c>
+      <c r="T7" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="V7" s="2" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:24" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:25" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
+        <v>43</v>
+      </c>
+      <c r="B8" t="s">
         <v>27</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="D8" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>30</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>31</v>
       </c>
-      <c r="I8" t="s">
+      <c r="J8" t="s">
         <v>32</v>
       </c>
-      <c r="J8" s="4">
+      <c r="K8" s="4">
         <v>40443</v>
       </c>
-      <c r="K8" s="4">
+      <c r="L8" s="4">
         <v>43167</v>
       </c>
-      <c r="L8" s="4"/>
-      <c r="M8" s="3">
+      <c r="M8" s="4"/>
+      <c r="N8" s="3">
         <v>43167</v>
       </c>
-      <c r="N8">
+      <c r="O8">
         <v>2</v>
       </c>
-      <c r="O8">
-        <v>0</v>
-      </c>
       <c r="P8">
         <v>0</v>
       </c>
       <c r="Q8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R8">
+        <v>1</v>
+      </c>
+      <c r="S8">
         <v>100</v>
       </c>
-      <c r="S8" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="U8" s="2" t="b">
+      <c r="T8" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="V8" s="2" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="J9" s="4"/>
+    <row r="9" spans="1:25" x14ac:dyDescent="0.35">
       <c r="K9" s="4"/>
       <c r="L9" s="4"/>
-      <c r="M9" s="3"/>
-      <c r="S9" s="2"/>
-      <c r="U9" s="2"/>
+      <c r="M9" s="4"/>
+      <c r="N9" s="3"/>
+      <c r="T9" s="2"/>
+      <c r="V9" s="2"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="C8" r:id="rId1" xr:uid="{796F2810-93EB-459F-9815-F3A57C0A19BB}"/>
-    <hyperlink ref="C4" r:id="rId2" xr:uid="{FDF72F62-9AC1-470E-B87E-AC09AAA46103}"/>
+    <hyperlink ref="D8" r:id="rId1" xr:uid="{796F2810-93EB-459F-9815-F3A57C0A19BB}"/>
+    <hyperlink ref="D4" r:id="rId2" xr:uid="{FDF72F62-9AC1-470E-B87E-AC09AAA46103}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
   <pageSetup orientation="portrait" r:id="rId3"/>

</xml_diff>